<commit_message>
update with SC worker range
</commit_message>
<xml_diff>
--- a/content/blog/2022/tanzu-avi-install/network-sheet.xlsx
+++ b/content/blog/2022/tanzu-avi-install/network-sheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/uhoelscher/Dev/everything-as-code/content/blog/2022/tanzu-avi-install/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCCA2F04-DB54-864D-B807-D79B9BC81D2B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{6EE6EE7C-9EEB-7E4A-BB5C-6E10E184DDB3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="38400" yWindow="500" windowWidth="38400" windowHeight="21100" xr2:uid="{618DF07D-69F4-914C-87C2-D538E33DF870}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
   <si>
     <t>DNS Server</t>
   </si>
@@ -134,6 +134,9 @@
   <si>
     <t>https://wp-content.vmware.com/v2/latest/lib.json</t>
   </si>
+  <si>
+    <t>Control Plane Starting IP</t>
+  </si>
 </sst>
 </file>
 
@@ -221,7 +224,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -229,6 +232,7 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -16010,13 +16014,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>101600</xdr:colOff>
-      <xdr:row>41</xdr:row>
+      <xdr:row>42</xdr:row>
       <xdr:rowOff>127000</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
       <xdr:colOff>1336632</xdr:colOff>
-      <xdr:row>42</xdr:row>
+      <xdr:row>43</xdr:row>
       <xdr:rowOff>130198</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -16350,10 +16354,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6EBE26F8-87DA-1A41-A132-D7295A12B886}">
-  <dimension ref="A1:B36"/>
+  <dimension ref="A1:B37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F26" sqref="F26"/>
+      <selection activeCell="B37" sqref="B37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -16390,7 +16394,7 @@
       <c r="A5" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="2"/>
+      <c r="B5" s="5"/>
     </row>
     <row r="6" spans="1:2" ht="19" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
@@ -16542,39 +16546,45 @@
     </row>
     <row r="32" spans="1:2" ht="19" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
-        <v>25</v>
+        <v>33</v>
       </c>
       <c r="B32" s="2"/>
     </row>
     <row r="33" spans="1:2" ht="19" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B33" s="2"/>
     </row>
     <row r="34" spans="1:2" ht="19" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B34" s="2"/>
+    </row>
+    <row r="35" spans="1:2" ht="19" x14ac:dyDescent="0.25">
+      <c r="A35" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="B34" s="3" t="s">
+      <c r="B35" s="3" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="35" spans="1:2" ht="19" x14ac:dyDescent="0.25">
-      <c r="A35" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="B35" s="2"/>
-    </row>
     <row r="36" spans="1:2" ht="19" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B36" s="2"/>
     </row>
+    <row r="37" spans="1:2" ht="19" x14ac:dyDescent="0.25">
+      <c r="A37" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B37" s="2"/>
+    </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B34" r:id="rId1" xr:uid="{C098D00A-91F3-5141-B4D1-350C5262E2DE}"/>
+    <hyperlink ref="B35" r:id="rId1" xr:uid="{C098D00A-91F3-5141-B4D1-350C5262E2DE}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId2"/>

</xml_diff>